<commit_message>
Update Coverage Tracker Excel with January 2026 Fingertip data
Updated all sheets with calculated values from raw Fingertip data:
- Executive Summary: Coverage metrics and top 15 plans
- Monthly Tracking: Jan-26 actual percentages and lives
- Charts: Updated chart data points
- Plan Detail: Top 10 covered plans with segments

Coverage Summary:
- Commercial: 7,034,139 / 187,209,835 = 3.76%
- Federal: 5,879,433 / 15,636,176 = 37.60%
- Medicare: 0 / 54,278,779 = 0.00%
- Medicaid: 0 / 73,287,278 = 0.00%

https://claude.ai/code/session_01NvMZkUTbijYBYidvnJA3Lx
</commit_message>
<xml_diff>
--- a/Cardamyst_Coverage_Tracker Jan 2026.xlsx
+++ b/Cardamyst_Coverage_Tracker Jan 2026.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Executive Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Monthly Tracking" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Charts" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Plan Detail" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Definitions" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Executive Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Monthly Tracking" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Charts" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plan Detail" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Definitions" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -312,14 +312,14 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -342,8 +342,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln w="0">
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -381,7 +381,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln w="47520">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="47520">
               <a:solidFill>
                 <a:srgbClr val="4A7EBB"/>
               </a:solidFill>
@@ -392,7 +392,7 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -521,7 +521,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln w="47520">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="47520">
               <a:solidFill>
                 <a:srgbClr val="BE4B48"/>
               </a:solidFill>
@@ -532,23 +532,23 @@
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <dLbls>
             <spPr>
-              <a:noFill/>
-              <a:ln>
+              <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:noFill/>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
             <txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
@@ -645,7 +645,7 @@
         </dLbls>
         <hiLowLines>
           <spPr>
-            <a:ln w="0">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -668,7 +668,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="9360">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9360">
             <a:solidFill>
               <a:srgbClr val="878787"/>
             </a:solidFill>
@@ -677,9 +677,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -712,7 +712,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln w="9360">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9360">
               <a:noFill/>
               <a:prstDash val="solid"/>
               <a:round/>
@@ -722,9 +722,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -747,8 +747,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill/>
-            <a:ln w="0">
+            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -759,7 +759,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="9360">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9360">
             <a:solidFill>
               <a:srgbClr val="878787"/>
             </a:solidFill>
@@ -768,9 +768,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -794,16 +794,16 @@
       <legendPos val="r"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln w="0">
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
@@ -823,10 +823,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill>
+    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
       <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
-    <a:ln w="9360">
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9360">
       <a:solidFill>
         <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
@@ -838,14 +838,14 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -868,8 +868,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln w="0">
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -896,10 +896,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="4F81BD"/>
             </a:solidFill>
-            <a:ln w="9360">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9360">
               <a:solidFill>
                 <a:srgbClr val="F9F9F9"/>
               </a:solidFill>
@@ -910,16 +910,16 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <spPr>
-              <a:noFill/>
-              <a:ln>
+              <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:noFill/>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
             <txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
@@ -999,7 +999,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="9360">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9360">
             <a:solidFill>
               <a:srgbClr val="878787"/>
             </a:solidFill>
@@ -1008,9 +1008,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1041,7 +1041,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln w="9360">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9360">
               <a:solidFill>
                 <a:srgbClr val="878787"/>
               </a:solidFill>
@@ -1053,9 +1053,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -1078,8 +1078,8 @@
           </tx>
           <overlay val="0"/>
           <spPr>
-            <a:noFill/>
-            <a:ln w="0">
+            <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -1090,7 +1090,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="9360">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9360">
             <a:solidFill>
               <a:srgbClr val="878787"/>
             </a:solidFill>
@@ -1099,9 +1099,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1125,16 +1125,16 @@
       <legendPos val="r"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln w="0">
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
@@ -1154,10 +1154,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill>
+    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
       <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
-    <a:ln w="9360">
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9360">
       <a:solidFill>
         <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
@@ -1169,7 +1169,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>7</col>
@@ -1189,9 +1189,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1216,9 +1216,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1463,20 +1463,14 @@
           <t>Segment</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>Total Lives</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Covered Lives</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>Coverage %</t>
-        </is>
+      <c r="B7" s="5" t="n">
+        <v>187209834</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>7034139</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.0376</v>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
@@ -1491,13 +1485,13 @@
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>187209834</v>
+        <v>15636175</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>7034139</v>
+        <v>5879432</v>
       </c>
       <c r="D8" s="8" t="n">
-        <v>0.03759999999999999</v>
+        <v>0.376</v>
       </c>
       <c r="E8" s="6" t="inlineStr">
         <is>
@@ -1512,13 +1506,13 @@
         </is>
       </c>
       <c r="B9" s="10" t="n">
-        <v>15636175</v>
+        <v>54278778</v>
       </c>
       <c r="C9" s="10" t="n">
-        <v>5879432</v>
+        <v>0</v>
       </c>
       <c r="D9" s="11" t="n">
-        <v>0.376</v>
+        <v>0</v>
       </c>
       <c r="E9" s="9" t="inlineStr">
         <is>
@@ -1533,7 +1527,7 @@
         </is>
       </c>
       <c r="B10" s="7" t="n">
-        <v>54278778</v>
+        <v>73287278</v>
       </c>
       <c r="C10" s="7" t="n">
         <v>0</v>
@@ -1554,13 +1548,13 @@
         </is>
       </c>
       <c r="B11" s="7" t="n">
-        <v>73287278</v>
+        <v>314775891</v>
       </c>
       <c r="C11" s="7" t="n">
-        <v>0</v>
+        <v>7034139</v>
       </c>
       <c r="D11" s="8" t="n">
-        <v>0</v>
+        <v>0.0223</v>
       </c>
       <c r="E11" s="6" t="inlineStr">
         <is>
@@ -1599,38 +1593,36 @@
     <row r="15">
       <c r="A15" s="16" t="inlineStr">
         <is>
-          <t>Plan Name</t>
+          <t>TRICARE Uniform Formulary</t>
         </is>
       </c>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>Plan Type</t>
-        </is>
-      </c>
-      <c r="C15" s="5" t="inlineStr">
-        <is>
-          <t>Covered Lives</t>
-        </is>
+          <t>Fed Prog</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>5879432.999999998</v>
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>Coverage Status</t>
+          <t>(T3)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
         <is>
-          <t>TRICARE Uniform Formulary</t>
+          <t>MGM Resorts International</t>
         </is>
       </c>
       <c r="B16" s="17" t="inlineStr">
         <is>
-          <t>Fed Prog</t>
+          <t>Employer</t>
         </is>
       </c>
       <c r="C16" s="18" t="n">
-        <v>5879432</v>
+        <v>185337</v>
       </c>
       <c r="D16" s="17" t="inlineStr">
         <is>
@@ -1641,47 +1633,47 @@
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>MGM Resorts International</t>
+          <t>UnitedHealthcare Community Plan Essential</t>
         </is>
       </c>
       <c r="B17" s="17" t="inlineStr">
         <is>
-          <t>Employer</t>
+          <t>HIX-Medicaid</t>
         </is>
       </c>
       <c r="C17" s="18" t="n">
-        <v>185337</v>
+        <v>174217</v>
       </c>
       <c r="D17" s="17" t="inlineStr">
         <is>
-          <t>(T3)</t>
+          <t>(T3)  (PA)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
-          <t>UnitedHealthcare Community Plan Essential</t>
+          <t>CHI Franciscan</t>
         </is>
       </c>
       <c r="B18" s="17" t="inlineStr">
         <is>
-          <t>HIX-Medicaid</t>
+          <t>Employer</t>
         </is>
       </c>
       <c r="C18" s="18" t="n">
-        <v>174217</v>
+        <v>135877</v>
       </c>
       <c r="D18" s="17" t="inlineStr">
         <is>
-          <t>(T3)  (PA)</t>
+          <t>(T3)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
         <is>
-          <t>CHI Franciscan</t>
+          <t>Apple</t>
         </is>
       </c>
       <c r="B19" s="17" t="inlineStr">
@@ -1690,7 +1682,7 @@
         </is>
       </c>
       <c r="C19" s="18" t="n">
-        <v>135877</v>
+        <v>118347</v>
       </c>
       <c r="D19" s="17" t="inlineStr">
         <is>
@@ -1701,7 +1693,7 @@
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>State of Ohio</t>
         </is>
       </c>
       <c r="B20" s="17" t="inlineStr">
@@ -1710,7 +1702,7 @@
         </is>
       </c>
       <c r="C20" s="18" t="n">
-        <v>118347</v>
+        <v>105536</v>
       </c>
       <c r="D20" s="17" t="inlineStr">
         <is>
@@ -1721,7 +1713,7 @@
     <row r="21">
       <c r="A21" s="6" t="inlineStr">
         <is>
-          <t>State of Ohio</t>
+          <t>General Electric</t>
         </is>
       </c>
       <c r="B21" s="17" t="inlineStr">
@@ -1730,7 +1722,7 @@
         </is>
       </c>
       <c r="C21" s="18" t="n">
-        <v>105536</v>
+        <v>98194</v>
       </c>
       <c r="D21" s="17" t="inlineStr">
         <is>
@@ -1741,7 +1733,7 @@
     <row r="22">
       <c r="A22" s="6" t="inlineStr">
         <is>
-          <t>General Electric</t>
+          <t>State of Michigan</t>
         </is>
       </c>
       <c r="B22" s="17" t="inlineStr">
@@ -1750,7 +1742,7 @@
         </is>
       </c>
       <c r="C22" s="18" t="n">
-        <v>98194</v>
+        <v>95690</v>
       </c>
       <c r="D22" s="17" t="inlineStr">
         <is>
@@ -1761,7 +1753,7 @@
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
         <is>
-          <t>State of Michigan</t>
+          <t>Weis Markets</t>
         </is>
       </c>
       <c r="B23" s="17" t="inlineStr">
@@ -1770,7 +1762,7 @@
         </is>
       </c>
       <c r="C23" s="18" t="n">
-        <v>95690</v>
+        <v>40010</v>
       </c>
       <c r="D23" s="17" t="inlineStr">
         <is>
@@ -1781,7 +1773,7 @@
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>Weis Markets</t>
+          <t>Smithfield Foods</t>
         </is>
       </c>
       <c r="B24" s="17" t="inlineStr">
@@ -1790,7 +1782,7 @@
         </is>
       </c>
       <c r="C24" s="18" t="n">
-        <v>40010</v>
+        <v>23040</v>
       </c>
       <c r="D24" s="17" t="inlineStr">
         <is>
@@ -1801,7 +1793,7 @@
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
         <is>
-          <t>Smithfield Foods</t>
+          <t>Milwaukee Public Schools</t>
         </is>
       </c>
       <c r="B25" s="17" t="inlineStr">
@@ -1810,7 +1802,7 @@
         </is>
       </c>
       <c r="C25" s="18" t="n">
-        <v>23040</v>
+        <v>20363</v>
       </c>
       <c r="D25" s="17" t="inlineStr">
         <is>
@@ -1830,11 +1822,11 @@
         </is>
       </c>
       <c r="C26" s="18" t="n">
-        <v>17009</v>
+        <v>16832</v>
       </c>
       <c r="D26" s="17" t="inlineStr">
         <is>
-          <t>(T3) Non-Preferred</t>
+          <t>(T3)</t>
         </is>
       </c>
     </row>
@@ -1850,11 +1842,11 @@
         </is>
       </c>
       <c r="C27" s="18" t="n">
-        <v>16004</v>
+        <v>15639</v>
       </c>
       <c r="D27" s="17" t="inlineStr">
         <is>
-          <t>(T3) Non-Preferred</t>
+          <t>(T3)</t>
         </is>
       </c>
     </row>
@@ -1870,11 +1862,11 @@
         </is>
       </c>
       <c r="C28" s="18" t="n">
-        <v>13977.3501852484</v>
+        <v>13977.35018524835</v>
       </c>
       <c r="D28" s="17" t="inlineStr">
         <is>
-          <t>(T3) Non-Preferred</t>
+          <t>(T3)</t>
         </is>
       </c>
     </row>
@@ -1890,11 +1882,11 @@
         </is>
       </c>
       <c r="C29" s="18" t="n">
-        <v>13631</v>
+        <v>13195</v>
       </c>
       <c r="D29" s="17" t="inlineStr">
         <is>
-          <t>(T3) Non-Preferred</t>
+          <t>(T3)</t>
         </is>
       </c>
     </row>
@@ -2055,7 +2047,7 @@
         </is>
       </c>
       <c r="B6" s="22" t="n">
-        <v>0</v>
+        <v>0.0376</v>
       </c>
       <c r="C6" s="22" t="n">
         <v>0</v>
@@ -2130,9 +2122,8 @@
           <t>Variance (pp)</t>
         </is>
       </c>
-      <c r="B8" s="24">
-        <f>IF(B7="","",(B7-B6))</f>
-        <v/>
+      <c r="B8" s="24" t="n">
+        <v>7034139</v>
       </c>
       <c r="C8" s="24">
         <f>IF(C7="","",(C7-C6))</f>
@@ -2198,7 +2189,7 @@
         </is>
       </c>
       <c r="B9" s="25" t="n">
-        <v>7034139</v>
+        <v>5879432</v>
       </c>
       <c r="C9" s="25" t="n"/>
       <c r="D9" s="25" t="n"/>
@@ -2252,10 +2243,8 @@
           <t>Month</t>
         </is>
       </c>
-      <c r="B13" s="5" t="inlineStr">
-        <is>
-          <t>Jan-26</t>
-        </is>
+      <c r="B13" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="C13" s="5" t="inlineStr">
         <is>
@@ -2389,10 +2378,8 @@
           <t>Month</t>
         </is>
       </c>
-      <c r="B18" s="5" t="inlineStr">
-        <is>
-          <t>Jan-26</t>
-        </is>
+      <c r="B18" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
@@ -2781,25 +2768,17 @@
           <t>Comm Forecast</t>
         </is>
       </c>
-      <c r="C3" s="31" t="inlineStr">
-        <is>
-          <t>Comm Actual</t>
-        </is>
-      </c>
-      <c r="D3" s="31" t="inlineStr">
-        <is>
-          <t>Medicare</t>
-        </is>
-      </c>
-      <c r="E3" s="31" t="inlineStr">
-        <is>
-          <t>Medicaid</t>
-        </is>
-      </c>
-      <c r="F3" s="31" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
+      <c r="C3" s="31" t="n">
+        <v>0.0376</v>
+      </c>
+      <c r="D3" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="31" t="n">
+        <v>0.0223</v>
       </c>
     </row>
     <row r="4">
@@ -3201,10 +3180,8 @@
           <t>Segment</t>
         </is>
       </c>
-      <c r="B23" s="4" t="inlineStr">
-        <is>
-          <t>Coverage %</t>
-        </is>
+      <c r="B23" s="4" t="n">
+        <v>0.037574</v>
       </c>
     </row>
     <row r="24">
@@ -3214,7 +3191,7 @@
         </is>
       </c>
       <c r="B24" s="33" t="n">
-        <v>0.0365448904718715</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -3250,7 +3227,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
@@ -3283,17 +3260,17 @@
     <row r="4">
       <c r="A4" s="21" t="inlineStr">
         <is>
-          <t>Segment</t>
+          <t>Commercial (Federal)</t>
         </is>
       </c>
       <c r="B4" s="21" t="inlineStr">
         <is>
-          <t>Plan Name</t>
+          <t>TRICARE Uniform Formulary</t>
         </is>
       </c>
       <c r="C4" s="21" t="inlineStr">
         <is>
-          <t>Plan Type</t>
+          <t>Fed Prog</t>
         </is>
       </c>
       <c r="D4" s="21" t="inlineStr">
@@ -3301,36 +3278,34 @@
           <t>Payer Name</t>
         </is>
       </c>
-      <c r="E4" s="21" t="inlineStr">
-        <is>
-          <t>Pharmacy Lives</t>
-        </is>
+      <c r="E4" s="21" t="n">
+        <v>5879432.999999998</v>
       </c>
       <c r="F4" s="21" t="inlineStr">
         <is>
-          <t>Coverage Status</t>
+          <t>(T3)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="36" t="inlineStr">
         <is>
-          <t>Commercial (Federal)</t>
+          <t>Commercial</t>
         </is>
       </c>
       <c r="B5" s="36" t="inlineStr">
         <is>
-          <t>TRICARE Uniform Formulary</t>
+          <t>MGM Resorts International</t>
         </is>
       </c>
       <c r="C5" s="36" t="inlineStr">
         <is>
-          <t>Fed Prog</t>
+          <t>Employer</t>
         </is>
       </c>
       <c r="D5" s="36" t="inlineStr"/>
       <c r="E5" s="37" t="n">
-        <v>5879432</v>
+        <v>185337</v>
       </c>
       <c r="F5" s="36" t="inlineStr">
         <is>
@@ -3346,47 +3321,47 @@
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>MGM Resorts International</t>
+          <t>UnitedHealthcare Community Plan Essential</t>
         </is>
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>Employer</t>
+          <t>HIX-Medicaid</t>
         </is>
       </c>
       <c r="D6" s="6" t="inlineStr"/>
       <c r="E6" s="7" t="n">
-        <v>185337</v>
+        <v>174217</v>
       </c>
       <c r="F6" s="6" t="inlineStr">
         <is>
-          <t>(T3)</t>
+          <t>(T3)  (PA)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>Medicaid</t>
+          <t>Commercial</t>
         </is>
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>UnitedHealthcare Community Plan Essential</t>
+          <t>CHI Franciscan</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>HIX-Medicaid</t>
+          <t>Employer</t>
         </is>
       </c>
       <c r="D7" s="6" t="inlineStr"/>
       <c r="E7" s="7" t="n">
-        <v>174217</v>
+        <v>135877</v>
       </c>
       <c r="F7" s="6" t="inlineStr">
         <is>
-          <t>(T3)  (PA)</t>
+          <t>(T3)</t>
         </is>
       </c>
     </row>
@@ -3398,7 +3373,7 @@
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
-          <t>CHI Franciscan</t>
+          <t>Apple</t>
         </is>
       </c>
       <c r="C8" s="6" t="inlineStr">
@@ -3408,7 +3383,7 @@
       </c>
       <c r="D8" s="6" t="inlineStr"/>
       <c r="E8" s="7" t="n">
-        <v>135877</v>
+        <v>118347</v>
       </c>
       <c r="F8" s="6" t="inlineStr">
         <is>
@@ -3424,7 +3399,7 @@
       </c>
       <c r="B9" s="6" t="inlineStr">
         <is>
-          <t>Apple</t>
+          <t>State of Ohio</t>
         </is>
       </c>
       <c r="C9" s="6" t="inlineStr">
@@ -3434,7 +3409,7 @@
       </c>
       <c r="D9" s="6" t="inlineStr"/>
       <c r="E9" s="7" t="n">
-        <v>118347</v>
+        <v>105536</v>
       </c>
       <c r="F9" s="6" t="inlineStr">
         <is>
@@ -3450,7 +3425,7 @@
       </c>
       <c r="B10" s="6" t="inlineStr">
         <is>
-          <t>State of Ohio</t>
+          <t>General Electric</t>
         </is>
       </c>
       <c r="C10" s="6" t="inlineStr">
@@ -3460,7 +3435,7 @@
       </c>
       <c r="D10" s="6" t="inlineStr"/>
       <c r="E10" s="7" t="n">
-        <v>105536</v>
+        <v>98194</v>
       </c>
       <c r="F10" s="6" t="inlineStr">
         <is>
@@ -3476,7 +3451,7 @@
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>General Electric</t>
+          <t>State of Michigan</t>
         </is>
       </c>
       <c r="C11" s="6" t="inlineStr">
@@ -3486,7 +3461,7 @@
       </c>
       <c r="D11" s="6" t="inlineStr"/>
       <c r="E11" s="7" t="n">
-        <v>98194</v>
+        <v>95690</v>
       </c>
       <c r="F11" s="6" t="inlineStr">
         <is>
@@ -3502,7 +3477,7 @@
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>State of Michigan</t>
+          <t>Weis Markets</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr">
@@ -3512,7 +3487,7 @@
       </c>
       <c r="D12" s="6" t="inlineStr"/>
       <c r="E12" s="7" t="n">
-        <v>95690</v>
+        <v>40010</v>
       </c>
       <c r="F12" s="6" t="inlineStr">
         <is>
@@ -3528,7 +3503,7 @@
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>Weis Markets</t>
+          <t>Smithfield Foods</t>
         </is>
       </c>
       <c r="C13" s="6" t="inlineStr">
@@ -3538,7 +3513,7 @@
       </c>
       <c r="D13" s="6" t="inlineStr"/>
       <c r="E13" s="7" t="n">
-        <v>40010</v>
+        <v>23040</v>
       </c>
       <c r="F13" s="6" t="inlineStr">
         <is>
@@ -3740,70 +3715,6 @@
       <c r="E35" s="7" t="n"/>
       <c r="F35" s="6" t="n"/>
     </row>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
-    <row r="53"/>
-    <row r="54"/>
-    <row r="55"/>
-    <row r="56"/>
-    <row r="57"/>
-    <row r="58"/>
-    <row r="59"/>
-    <row r="60"/>
-    <row r="61"/>
-    <row r="62"/>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70"/>
-    <row r="71"/>
-    <row r="72"/>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88"/>
-    <row r="89"/>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92"/>
-    <row r="93"/>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98"/>
-    <row r="99"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>